<commit_message>
updated inshore raw data
</commit_message>
<xml_diff>
--- a/data/PAM/2021-06-08_Past-4temps-Inshore.xlsx
+++ b/data/PAM/2021-06-08_Past-4temps-Inshore.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="147">
   <si>
     <t>TubeNumber</t>
   </si>
@@ -461,7 +461,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -484,6 +484,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -499,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -524,6 +529,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9889,6 +9897,826 @@
         <v>44356.0</v>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C212" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E212" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F212" s="4">
+        <v>36.0</v>
+      </c>
+      <c r="G212" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H212" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I212" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="J212" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L212" s="9">
+        <v>0.583</v>
+      </c>
+      <c r="M212" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N212" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C213" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E213" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F213" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="G213" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H213" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I213" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="J213" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L213" s="9">
+        <v>0.613</v>
+      </c>
+      <c r="M213" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N213" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C214" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E214" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F214" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="G214" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H214" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I214" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="J214" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L214" s="9">
+        <v>0.623</v>
+      </c>
+      <c r="M214" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N214" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C215" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F215" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="G215" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H215" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I215" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="J215" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L215" s="9">
+        <v>0.603</v>
+      </c>
+      <c r="M215" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N215" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C216" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F216" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G216" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H216" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I216" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="J216" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L216" s="9">
+        <v>0.549</v>
+      </c>
+      <c r="M216" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N216" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C217" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E217" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F217" s="4">
+        <v>36.0</v>
+      </c>
+      <c r="G217" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H217" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I217" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="J217" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L217" s="9">
+        <v>0.613</v>
+      </c>
+      <c r="M217" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N217" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C218" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E218" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F218" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="G218" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H218" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I218" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="J218" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L218" s="9">
+        <v>0.596</v>
+      </c>
+      <c r="M218" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N218" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C219" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E219" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F219" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="G219" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H219" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I219" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="J219" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L219" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="M219" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N219" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C220" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E220" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F220" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="G220" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H220" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I220" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="J220" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L220" s="9">
+        <v>0.604</v>
+      </c>
+      <c r="M220" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N220" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C221" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E221" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F221" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G221" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H221" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I221" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="J221" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L221" s="9">
+        <v>0.591</v>
+      </c>
+      <c r="M221" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N221" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C222" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E222" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F222" s="4">
+        <v>36.0</v>
+      </c>
+      <c r="G222" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H222" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I222" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="J222" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L222" s="9">
+        <v>0.429</v>
+      </c>
+      <c r="M222" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N222" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C223" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E223" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F223" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="G223" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H223" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I223" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="J223" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L223" s="9">
+        <v>0.533</v>
+      </c>
+      <c r="M223" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N223" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C224" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D224" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E224" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F224" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="G224" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H224" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I224" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="J224" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L224" s="9">
+        <v>0.539</v>
+      </c>
+      <c r="M224" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N224" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C225" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F225" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="G225" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I225" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="J225" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L225" s="9">
+        <v>0.349</v>
+      </c>
+      <c r="M225" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N225" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C226" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F226" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G226" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H226" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I226" s="4">
+        <v>37.0</v>
+      </c>
+      <c r="J226" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L226" s="9">
+        <v>0.408</v>
+      </c>
+      <c r="M226" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N226" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C227" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E227" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F227" s="4">
+        <v>36.0</v>
+      </c>
+      <c r="G227" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H227" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I227" s="4">
+        <v>39.0</v>
+      </c>
+      <c r="J227" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L227" s="9">
+        <v>0.051</v>
+      </c>
+      <c r="M227" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N227" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C228" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E228" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F228" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="G228" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H228" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I228" s="4">
+        <v>39.0</v>
+      </c>
+      <c r="J228" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L228" s="9">
+        <v>0.128</v>
+      </c>
+      <c r="M228" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N228" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C229" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E229" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F229" s="4">
+        <v>38.0</v>
+      </c>
+      <c r="G229" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H229" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I229" s="4">
+        <v>39.0</v>
+      </c>
+      <c r="J229" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L229" s="9">
+        <v>0.069</v>
+      </c>
+      <c r="M229" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N229" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C230" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E230" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F230" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="G230" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H230" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I230" s="4">
+        <v>39.0</v>
+      </c>
+      <c r="J230" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L230" s="9">
+        <v>0.104</v>
+      </c>
+      <c r="M230" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N230" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C231" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E231" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F231" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G231" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H231" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I231" s="4">
+        <v>39.0</v>
+      </c>
+      <c r="J231" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="L231" s="9">
+        <v>0.027</v>
+      </c>
+      <c r="M231" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N231" s="6">
+        <v>44355.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>